<commit_message>
Fuels report creation and corrected names
</commit_message>
<xml_diff>
--- a/Costs/fuels/tables/FuelsAnalysis.xlsx
+++ b/Costs/fuels/tables/FuelsAnalysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldo\Documents\Facultad\Internship Berkeley\Análisis de datos\switch_mexico_data\Costs\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldo\Documents\Facultad\Internship Berkeley\Análisis de datos\switch_mexico_data\Costs\fuels\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="national fuel oil" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Diesel Nacional</t>
   </si>
   <si>
-    <t>Diesel Pennsula de Yucatan</t>
-  </si>
-  <si>
     <t>Domestic natural gas; Dos Bocas, Veracruz</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t>imported fuel oil</t>
+  </si>
+  <si>
+    <t>Diesel Peninsula de Yucatan</t>
   </si>
 </sst>
 </file>
@@ -1044,67 +1044,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" t="s">
-        <v>50</v>
-      </c>
       <c r="U1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -2164,52 +2164,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="P1" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -2217,49 +2217,49 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" t="s">
-        <v>39</v>
-      </c>
       <c r="P2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -3021,24 +3021,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3052,7 +3052,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3285,16 +3285,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3308,7 +3308,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3530,7 +3530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B17"/>
     </sheetView>
   </sheetViews>
@@ -3538,10 +3538,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3549,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3689,10 +3689,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3700,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3840,10 +3840,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3851,7 +3851,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3991,10 +3991,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fuel's cost report finished
</commit_message>
<xml_diff>
--- a/Costs/fuels/tables/FuelsAnalysis.xlsx
+++ b/Costs/fuels/tables/FuelsAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="national fuel oil" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,15 @@
     <sheet name="diesel" sheetId="3" r:id="rId3"/>
     <sheet name="carbon" sheetId="4" r:id="rId4"/>
     <sheet name="uranium" sheetId="6" r:id="rId5"/>
-    <sheet name="liquified natural gas" sheetId="8" r:id="rId6"/>
-    <sheet name="imported natural gas" sheetId="9" r:id="rId7"/>
-    <sheet name="imported fuel oil" sheetId="10" r:id="rId8"/>
+    <sheet name="imported natural gas" sheetId="9" r:id="rId6"/>
+    <sheet name="imported fuel oil" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Year</t>
   </si>
@@ -2154,15 +2153,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2211,8 +2210,11 @@
       <c r="P1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2261,8 +2263,11 @@
       <c r="P2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -2311,8 +2316,11 @@
       <c r="P3">
         <v>4.7755802139999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <v>3.7762802139999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -2361,8 +2369,11 @@
       <c r="P4">
         <v>5.2720286649999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>4.2727286649999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -2411,8 +2422,11 @@
       <c r="P5">
         <v>5.1642419009999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>4.1649419009999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -2461,8 +2475,11 @@
       <c r="P6">
         <v>5.3891843740000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>4.3898843740000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -2511,8 +2528,11 @@
       <c r="P7">
         <v>5.5074772269999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>4.508177227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -2561,8 +2581,11 @@
       <c r="P8">
         <v>5.6118380119999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <v>4.6125380119999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -2611,8 +2634,11 @@
       <c r="P9">
         <v>5.7161983139999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>4.7168983139999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -2661,8 +2687,11 @@
       <c r="P10">
         <v>5.7683784649999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <v>4.7690784649999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2024</v>
       </c>
@@ -2711,8 +2740,11 @@
       <c r="P11">
         <v>5.8205590989999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <v>4.8212590989999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2025</v>
       </c>
@@ -2761,8 +2793,11 @@
       <c r="P12">
         <v>5.8727392500000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <v>4.8734392499999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2026</v>
       </c>
@@ -2811,8 +2846,11 @@
       <c r="P13">
         <v>5.9249198840000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <v>4.9256198839999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2027</v>
       </c>
@@ -2861,8 +2899,11 @@
       <c r="P14">
         <v>5.9771005180000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>4.9778005179999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2028</v>
       </c>
@@ -2911,8 +2952,11 @@
       <c r="P15">
         <v>6.0292801860000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <v>5.0299801860000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2029</v>
       </c>
@@ -2961,8 +3005,11 @@
       <c r="P16">
         <v>6.0814608200000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>5.0821608200000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2030</v>
       </c>
@@ -3010,6 +3057,9 @@
       </c>
       <c r="P17">
         <v>6.1336409710000002</v>
+      </c>
+      <c r="Q17">
+        <v>5.1343409710000003</v>
       </c>
     </row>
   </sheetData>
@@ -3021,7 +3071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3681,7 +3731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3700,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3708,7 +3758,7 @@
         <v>2016</v>
       </c>
       <c r="B3">
-        <v>3.7762802139999998</v>
+        <v>4.7251454920000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3716,7 +3766,7 @@
         <v>2017</v>
       </c>
       <c r="B4">
-        <v>4.2727286649999998</v>
+        <v>5.3026898989999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3724,7 +3774,7 @@
         <v>2018</v>
       </c>
       <c r="B5">
-        <v>4.1649419009999997</v>
+        <v>5.185616317</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3732,7 +3782,7 @@
         <v>2019</v>
       </c>
       <c r="B6">
-        <v>4.3898843740000002</v>
+        <v>5.4473036429999997</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3740,7 +3790,7 @@
         <v>2020</v>
       </c>
       <c r="B7">
-        <v>4.508177227</v>
+        <v>5.5849198949999996</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3748,7 +3798,7 @@
         <v>2021</v>
       </c>
       <c r="B8">
-        <v>4.6125380119999999</v>
+        <v>5.706328246</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3756,7 +3806,7 @@
         <v>2022</v>
       </c>
       <c r="B9">
-        <v>4.7168983139999998</v>
+        <v>5.827736034</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3764,7 +3814,7 @@
         <v>2023</v>
       </c>
       <c r="B10">
-        <v>4.7690784649999998</v>
+        <v>5.8884399289999996</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3772,7 +3822,7 @@
         <v>2024</v>
       </c>
       <c r="B11">
-        <v>4.8212590989999997</v>
+        <v>5.9491443850000003</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3780,7 +3830,7 @@
         <v>2025</v>
       </c>
       <c r="B12">
-        <v>4.8734392499999997</v>
+        <v>6.0098482789999998</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3788,7 +3838,7 @@
         <v>2026</v>
       </c>
       <c r="B13">
-        <v>4.9256198839999996</v>
+        <v>6.0705527359999998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -3796,7 +3846,7 @@
         <v>2027</v>
       </c>
       <c r="B14">
-        <v>4.9778005179999996</v>
+        <v>6.1312571919999996</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3804,7 +3854,7 @@
         <v>2028</v>
       </c>
       <c r="B15">
-        <v>5.0299801860000004</v>
+        <v>6.1919605239999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3812,7 +3862,7 @@
         <v>2029</v>
       </c>
       <c r="B16">
-        <v>5.0821608200000004</v>
+        <v>6.2526649809999997</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3820,7 +3870,7 @@
         <v>2030</v>
       </c>
       <c r="B17">
-        <v>5.1343409710000003</v>
+        <v>6.3133688750000001</v>
       </c>
     </row>
   </sheetData>
@@ -3851,157 +3901,6 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2016</v>
-      </c>
-      <c r="B3">
-        <v>4.7251454920000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2017</v>
-      </c>
-      <c r="B4">
-        <v>5.3026898989999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2018</v>
-      </c>
-      <c r="B5">
-        <v>5.185616317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2019</v>
-      </c>
-      <c r="B6">
-        <v>5.4473036429999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2020</v>
-      </c>
-      <c r="B7">
-        <v>5.5849198949999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2021</v>
-      </c>
-      <c r="B8">
-        <v>5.706328246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2022</v>
-      </c>
-      <c r="B9">
-        <v>5.827736034</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2023</v>
-      </c>
-      <c r="B10">
-        <v>5.8884399289999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2024</v>
-      </c>
-      <c r="B11">
-        <v>5.9491443850000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2025</v>
-      </c>
-      <c r="B12">
-        <v>6.0098482789999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2026</v>
-      </c>
-      <c r="B13">
-        <v>6.0705527359999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2027</v>
-      </c>
-      <c r="B14">
-        <v>6.1312571919999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2028</v>
-      </c>
-      <c r="B15">
-        <v>6.1919605239999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2029</v>
-      </c>
-      <c r="B16">
-        <v>6.2526649809999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2030</v>
-      </c>
-      <c r="B17">
-        <v>6.3133688750000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>